<commit_message>
Update brain hotspot positions and add brain region info to popup
- Update all hotspot coordinates from brain_regions.xlsx
- Add corresponding brain region to each hotspot (Occipital Lobe, Auditory cortex, etc.)
- Display brain region in popup when clicking from Brain Regions UI

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/brain_regions.xlsx
+++ b/brain_regions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cobyp\3d-brain\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cobyp\cobypal-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04724EFE-6542-4CB6-8CC6-3B4EC4E5502A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4BE4F4-EB28-4DBC-8009-29000721674E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="38610" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>BRAIN REGION</t>
   </si>
@@ -85,31 +85,61 @@
     <t>Default Coordinates</t>
   </si>
   <si>
-    <t>THREE.Vector3(-45.51, -20.94, -31.85)</t>
-  </si>
-  <si>
-    <t>THREE.Vector3(-47.86, -4.89, 11.82)</t>
-  </si>
-  <si>
-    <t>THREE.Vector3(-38.79, 7.22, 46.75)</t>
-  </si>
-  <si>
-    <t>THREE.Vector3(-29.30, 19.57, 60.03)</t>
-  </si>
-  <si>
-    <t>THREE.Vector3(-52.49, -3.26, -12.82)</t>
-  </si>
-  <si>
-    <t>THREE.Vector3(-36.94, 14.21, -53.12)</t>
-  </si>
-  <si>
-    <t>THREE.Vector3(-34.23, 29.35, 28.31)</t>
-  </si>
-  <si>
-    <t>THREE.Vector3(-13.00, 34.80, 59.41)</t>
-  </si>
-  <si>
-    <t>THREE.Vector3(-52.97, 23.33, -22.01)</t>
+    <t>Occipital Lobe</t>
+  </si>
+  <si>
+    <t>Auditory cortex</t>
+  </si>
+  <si>
+    <t>Motor cortex</t>
+  </si>
+  <si>
+    <t>Hypothalamus</t>
+  </si>
+  <si>
+    <t>Cerebellum</t>
+  </si>
+  <si>
+    <t>Corresponding Brain Region</t>
+  </si>
+  <si>
+    <t>Temporal language areas (Wernicke’s area)</t>
+  </si>
+  <si>
+    <t>Dorsolateral prefrontal cortex</t>
+  </si>
+  <si>
+    <t>Ventromedial prefrontal cortex</t>
+  </si>
+  <si>
+    <t>Anterior prefrontal cortex</t>
+  </si>
+  <si>
+    <t>THREE.Vector3(-48.33, -31.49, -23.14)</t>
+  </si>
+  <si>
+    <t>THREE.Vector3(-15.16, -28.65, 1.76)</t>
+  </si>
+  <si>
+    <t>THREE.Vector3(38.62, 21.26, 40.53)</t>
+  </si>
+  <si>
+    <t>THREE.Vector3(-11.15, 47.78, 38.80)</t>
+  </si>
+  <si>
+    <t>THREE.Vector3(31.93, 45.64, 12.26)</t>
+  </si>
+  <si>
+    <t>THREE.Vector3(-55.86, 9.78, -3.42)</t>
+  </si>
+  <si>
+    <t>THREE.Vector3(53.49, 15.30, -18.65)</t>
+  </si>
+  <si>
+    <t>THREE.Vector3(-15.55, 20.11, 67.40)</t>
+  </si>
+  <si>
+    <t>THREE.Vector3(-30.06, 4.40, -59.25)</t>
   </si>
 </sst>
 </file>
@@ -382,19 +412,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.7109375" customWidth="1"/>
     <col min="2" max="2" width="44" customWidth="1"/>
+    <col min="3" max="3" width="58.28515625" customWidth="1"/>
+    <col min="4" max="4" width="44.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -404,8 +436,11 @@
       <c r="C1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -413,10 +448,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -424,10 +462,13 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -435,10 +476,13 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -446,10 +490,13 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -457,10 +504,13 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -468,10 +518,13 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -479,10 +532,13 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -490,10 +546,13 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -501,7 +560,10 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>